<commit_message>
Got new data from FRP
</commit_message>
<xml_diff>
--- a/FRP_EMPcrosswalk.xlsx
+++ b/FRP_EMPcrosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/ZoopAnalyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="11_D1D8BACF3E4A32804D628C8F00905AC72DA55AA6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{621F99CA-0BF3-467F-8B8D-E34152CAE14C}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="11_D1D8BACF3E4A32804D628C8F00905AC72DA55AA6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{65A613F8-C2D1-44DC-B2B6-1FACEE1CF9DB}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zoopsonly" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3275" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3023" uniqueCount="579">
   <si>
     <t>ACARTELA</t>
   </si>
@@ -1824,9 +1824,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Adult</t>
   </si>
   <si>
@@ -1905,12 +1902,6 @@
     <t>Subclass</t>
   </si>
   <si>
-    <t>OTHCOPNAUP</t>
-  </si>
-  <si>
-    <t>PDIAPNAUP</t>
-  </si>
-  <si>
     <t>Branchiopoda</t>
   </si>
   <si>
@@ -2014,6 +2005,30 @@
   </si>
   <si>
     <t>Analy2</t>
+  </si>
+  <si>
+    <t>BOSMI</t>
+  </si>
+  <si>
+    <t>EURYUP</t>
+  </si>
+  <si>
+    <t>PDIAPUP</t>
+  </si>
+  <si>
+    <t>SINOUP</t>
+  </si>
+  <si>
+    <t>AVERL</t>
+  </si>
+  <si>
+    <t>COPUP</t>
+  </si>
+  <si>
+    <t>OTHCOPUP</t>
+  </si>
+  <si>
+    <t>BARNUP</t>
   </si>
 </sst>
 </file>
@@ -5020,7 +5035,7 @@
   <dimension ref="A1:R119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P115" sqref="P115"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5069,24 +5084,12 @@
         <v>422</v>
       </c>
       <c r="L1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>510</v>
-      </c>
-      <c r="B2" t="s">
-        <v>510</v>
-      </c>
-      <c r="C2" t="s">
-        <v>510</v>
-      </c>
-      <c r="D2" t="s">
-        <v>510</v>
-      </c>
       <c r="E2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F2" t="s">
         <v>215</v>
@@ -5095,10 +5098,10 @@
         <v>506</v>
       </c>
       <c r="H2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J2" t="s">
         <v>215</v>
@@ -5114,10 +5117,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>571</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>571</v>
       </c>
       <c r="C3" t="s">
         <v>136</v>
@@ -5126,7 +5129,7 @@
         <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F3" t="s">
         <v>63</v>
@@ -5135,10 +5138,10 @@
         <v>509</v>
       </c>
       <c r="H3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I3" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J3" t="s">
         <v>215</v>
@@ -5164,7 +5167,7 @@
         <v>137</v>
       </c>
       <c r="E4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F4" t="s">
         <v>137</v>
@@ -5173,10 +5176,10 @@
         <v>508</v>
       </c>
       <c r="H4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I4" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J4" t="s">
         <v>215</v>
@@ -5204,7 +5207,7 @@
         <v>140</v>
       </c>
       <c r="E5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F5" t="s">
         <v>140</v>
@@ -5213,10 +5216,10 @@
         <v>508</v>
       </c>
       <c r="H5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I5" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J5" t="s">
         <v>215</v>
@@ -5229,12 +5232,6 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>510</v>
-      </c>
-      <c r="B6" t="s">
-        <v>510</v>
-      </c>
       <c r="C6" t="s">
         <v>138</v>
       </c>
@@ -5242,7 +5239,7 @@
         <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F6" t="s">
         <v>138</v>
@@ -5251,10 +5248,10 @@
         <v>508</v>
       </c>
       <c r="H6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I6" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J6" t="s">
         <v>215</v>
@@ -5269,12 +5266,6 @@
       <c r="Q6" s="75"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>510</v>
-      </c>
-      <c r="B7" t="s">
-        <v>510</v>
-      </c>
       <c r="C7" t="s">
         <v>487</v>
       </c>
@@ -5282,7 +5273,7 @@
         <v>215</v>
       </c>
       <c r="E7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F7" t="s">
         <v>215</v>
@@ -5291,10 +5282,10 @@
         <v>506</v>
       </c>
       <c r="H7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I7" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J7" t="s">
         <v>215</v>
@@ -5322,7 +5313,7 @@
         <v>139</v>
       </c>
       <c r="E8" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F8" t="s">
         <v>215</v>
@@ -5331,10 +5322,10 @@
         <v>506</v>
       </c>
       <c r="H8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I8" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J8" t="s">
         <v>215</v>
@@ -5351,20 +5342,11 @@
       <c r="R8" s="75"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>510</v>
-      </c>
-      <c r="B9" t="s">
-        <v>510</v>
-      </c>
-      <c r="C9" t="s">
-        <v>510</v>
-      </c>
       <c r="D9" t="s">
         <v>267</v>
       </c>
       <c r="E9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F9" t="s">
         <v>267</v>
@@ -5373,10 +5355,10 @@
         <v>508</v>
       </c>
       <c r="H9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I9" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J9" t="s">
         <v>215</v>
@@ -5390,32 +5372,23 @@
       <c r="N9" s="75"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10" t="s">
+        <v>547</v>
+      </c>
+      <c r="E10" t="s">
         <v>510</v>
       </c>
-      <c r="B10" t="s">
-        <v>510</v>
-      </c>
-      <c r="C10" t="s">
-        <v>510</v>
-      </c>
-      <c r="D10" t="s">
-        <v>550</v>
-      </c>
-      <c r="E10" t="s">
-        <v>511</v>
-      </c>
       <c r="F10" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="G10" t="s">
         <v>508</v>
       </c>
       <c r="H10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I10" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J10" t="s">
         <v>215</v>
@@ -5430,20 +5403,11 @@
       <c r="P10" s="75"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>510</v>
-      </c>
-      <c r="B11" t="s">
-        <v>510</v>
-      </c>
-      <c r="C11" t="s">
-        <v>510</v>
-      </c>
       <c r="D11" t="s">
         <v>253</v>
       </c>
       <c r="E11" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F11" t="s">
         <v>253</v>
@@ -5452,10 +5416,10 @@
         <v>507</v>
       </c>
       <c r="H11" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I11" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J11" t="s">
         <v>215</v>
@@ -5470,20 +5434,11 @@
       <c r="P11" s="75"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>510</v>
-      </c>
-      <c r="B12" t="s">
-        <v>510</v>
-      </c>
-      <c r="C12" t="s">
-        <v>510</v>
-      </c>
       <c r="D12" t="s">
         <v>268</v>
       </c>
       <c r="E12" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F12" t="s">
         <v>268</v>
@@ -5492,10 +5447,10 @@
         <v>508</v>
       </c>
       <c r="H12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I12" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J12" t="s">
         <v>215</v>
@@ -5510,20 +5465,11 @@
       <c r="P12" s="75"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>510</v>
-      </c>
-      <c r="B13" t="s">
-        <v>510</v>
-      </c>
-      <c r="C13" t="s">
-        <v>510</v>
-      </c>
       <c r="D13" t="s">
         <v>255</v>
       </c>
       <c r="E13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F13" t="s">
         <v>255</v>
@@ -5532,10 +5478,10 @@
         <v>508</v>
       </c>
       <c r="H13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I13" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J13" t="s">
         <v>215</v>
@@ -5550,20 +5496,11 @@
       <c r="P13" s="75"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>510</v>
-      </c>
-      <c r="B14" t="s">
-        <v>510</v>
-      </c>
-      <c r="C14" t="s">
-        <v>510</v>
-      </c>
       <c r="D14" t="s">
         <v>251</v>
       </c>
       <c r="E14" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F14" t="s">
         <v>251</v>
@@ -5572,10 +5509,10 @@
         <v>508</v>
       </c>
       <c r="H14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I14" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J14" t="s">
         <v>215</v>
@@ -5589,20 +5526,11 @@
       <c r="P14" s="75"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>510</v>
-      </c>
-      <c r="B15" t="s">
-        <v>510</v>
-      </c>
-      <c r="C15" t="s">
-        <v>510</v>
-      </c>
       <c r="D15" t="s">
         <v>242</v>
       </c>
       <c r="E15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F15" t="s">
         <v>242</v>
@@ -5611,10 +5539,10 @@
         <v>508</v>
       </c>
       <c r="H15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I15" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J15" t="s">
         <v>215</v>
@@ -5627,20 +5555,11 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>510</v>
-      </c>
-      <c r="B16" t="s">
-        <v>510</v>
-      </c>
-      <c r="C16" t="s">
-        <v>510</v>
-      </c>
       <c r="D16" t="s">
         <v>238</v>
       </c>
       <c r="E16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F16" t="s">
         <v>238</v>
@@ -5649,10 +5568,10 @@
         <v>508</v>
       </c>
       <c r="H16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I16" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J16" t="s">
         <v>215</v>
@@ -5667,20 +5586,11 @@
       <c r="P16" s="75"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>510</v>
-      </c>
-      <c r="B17" t="s">
-        <v>510</v>
-      </c>
-      <c r="C17" t="s">
-        <v>510</v>
-      </c>
       <c r="D17" t="s">
         <v>269</v>
       </c>
       <c r="E17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F17" t="s">
         <v>269</v>
@@ -5689,10 +5599,10 @@
         <v>508</v>
       </c>
       <c r="H17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I17" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J17" t="s">
         <v>215</v>
@@ -5705,20 +5615,11 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>510</v>
-      </c>
-      <c r="B18" t="s">
-        <v>510</v>
-      </c>
-      <c r="C18" t="s">
-        <v>510</v>
-      </c>
       <c r="D18" t="s">
         <v>214</v>
       </c>
       <c r="E18" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F18" t="s">
         <v>214</v>
@@ -5727,10 +5628,10 @@
         <v>508</v>
       </c>
       <c r="H18" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I18" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J18" t="s">
         <v>215</v>
@@ -5745,32 +5646,20 @@
       <c r="P18" s="75"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E19" t="s">
         <v>510</v>
       </c>
-      <c r="B19" t="s">
-        <v>510</v>
-      </c>
-      <c r="C19" t="s">
-        <v>510</v>
-      </c>
-      <c r="D19" t="s">
-        <v>510</v>
-      </c>
-      <c r="E19" t="s">
-        <v>511</v>
-      </c>
       <c r="F19" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="G19" t="s">
         <v>509</v>
       </c>
       <c r="H19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I19" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J19" t="s">
         <v>215</v>
@@ -5785,32 +5674,20 @@
       <c r="P19" s="75"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E20" t="s">
         <v>510</v>
       </c>
-      <c r="B20" t="s">
-        <v>510</v>
-      </c>
-      <c r="C20" t="s">
-        <v>510</v>
-      </c>
-      <c r="D20" t="s">
-        <v>510</v>
-      </c>
-      <c r="E20" t="s">
-        <v>511</v>
-      </c>
       <c r="F20" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="G20" t="s">
         <v>509</v>
       </c>
       <c r="H20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I20" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J20" t="s">
         <v>215</v>
@@ -5838,7 +5715,7 @@
         <v>142</v>
       </c>
       <c r="E21" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F21" t="s">
         <v>1</v>
@@ -5847,16 +5724,16 @@
         <v>509</v>
       </c>
       <c r="H21" t="s">
+        <v>511</v>
+      </c>
+      <c r="I21" t="s">
         <v>512</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>513</v>
       </c>
-      <c r="J21" t="s">
-        <v>514</v>
-      </c>
       <c r="K21" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L21" t="s">
         <v>142</v>
@@ -5878,68 +5755,59 @@
         <v>141</v>
       </c>
       <c r="E22" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F22" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G22" t="s">
         <v>508</v>
       </c>
       <c r="H22" t="s">
+        <v>511</v>
+      </c>
+      <c r="I22" t="s">
         <v>512</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>513</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
+        <v>513</v>
+      </c>
+      <c r="L22" t="s">
         <v>514</v>
-      </c>
-      <c r="K22" t="s">
-        <v>514</v>
-      </c>
-      <c r="L22" t="s">
-        <v>515</v>
       </c>
       <c r="N22" s="75"/>
       <c r="P22" s="75"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>510</v>
-      </c>
-      <c r="B23" t="s">
-        <v>510</v>
-      </c>
       <c r="C23" t="s">
         <v>492</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>510</v>
       </c>
-      <c r="E23" t="s">
-        <v>511</v>
-      </c>
       <c r="F23" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G23" t="s">
         <v>508</v>
       </c>
       <c r="H23" t="s">
+        <v>511</v>
+      </c>
+      <c r="I23" t="s">
         <v>512</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>513</v>
       </c>
-      <c r="J23" t="s">
-        <v>514</v>
-      </c>
       <c r="K23" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L23" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P23" s="75"/>
     </row>
@@ -5950,14 +5818,11 @@
       <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="C24" t="s">
-        <v>510</v>
-      </c>
       <c r="D24" t="s">
         <v>225</v>
       </c>
       <c r="E24" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F24" t="s">
         <v>5</v>
@@ -5966,19 +5831,19 @@
         <v>507</v>
       </c>
       <c r="H24" t="s">
+        <v>511</v>
+      </c>
+      <c r="I24" t="s">
         <v>512</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>513</v>
       </c>
-      <c r="J24" t="s">
-        <v>514</v>
-      </c>
       <c r="K24" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L24" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N24" s="75"/>
     </row>
@@ -5996,7 +5861,7 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F25" t="s">
         <v>7</v>
@@ -6005,30 +5870,24 @@
         <v>509</v>
       </c>
       <c r="H25" t="s">
+        <v>511</v>
+      </c>
+      <c r="I25" t="s">
         <v>512</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>513</v>
       </c>
-      <c r="J25" t="s">
-        <v>514</v>
-      </c>
       <c r="K25" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L25" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N25" s="75"/>
       <c r="P25" s="75"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>510</v>
-      </c>
-      <c r="B26" t="s">
-        <v>510</v>
-      </c>
       <c r="C26" t="s">
         <v>190</v>
       </c>
@@ -6036,25 +5895,25 @@
         <v>190</v>
       </c>
       <c r="E26" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F26" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G26" t="s">
         <v>509</v>
       </c>
       <c r="H26" t="s">
+        <v>511</v>
+      </c>
+      <c r="I26" t="s">
         <v>512</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>513</v>
       </c>
-      <c r="J26" t="s">
-        <v>514</v>
-      </c>
       <c r="K26" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L26" t="s">
         <v>190</v>
@@ -6062,12 +5921,6 @@
       <c r="P26" s="75"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>510</v>
-      </c>
-      <c r="B27" t="s">
-        <v>510</v>
-      </c>
       <c r="C27" t="s">
         <v>486</v>
       </c>
@@ -6075,25 +5928,25 @@
         <v>152</v>
       </c>
       <c r="E27" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F27" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G27" t="s">
         <v>506</v>
       </c>
       <c r="H27" t="s">
+        <v>511</v>
+      </c>
+      <c r="I27" t="s">
         <v>512</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>513</v>
       </c>
-      <c r="J27" t="s">
-        <v>514</v>
-      </c>
       <c r="K27" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L27" t="s">
         <v>151</v>
@@ -6101,38 +5954,29 @@
       <c r="N27" s="75"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>510</v>
-      </c>
-      <c r="B28" t="s">
-        <v>510</v>
-      </c>
-      <c r="C28" t="s">
-        <v>510</v>
-      </c>
       <c r="D28" t="s">
         <v>294</v>
       </c>
       <c r="E28" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G28" t="s">
         <v>506</v>
       </c>
       <c r="H28" t="s">
+        <v>511</v>
+      </c>
+      <c r="I28" t="s">
         <v>512</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>513</v>
       </c>
-      <c r="J28" t="s">
-        <v>514</v>
-      </c>
       <c r="K28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L28" t="s">
         <v>151</v>
@@ -6154,25 +5998,25 @@
         <v>151</v>
       </c>
       <c r="E29" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F29" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G29" t="s">
         <v>506</v>
       </c>
       <c r="H29" t="s">
+        <v>511</v>
+      </c>
+      <c r="I29" t="s">
         <v>512</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>513</v>
       </c>
-      <c r="J29" t="s">
-        <v>514</v>
-      </c>
       <c r="K29" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L29" t="s">
         <v>151</v>
@@ -6181,12 +6025,6 @@
       <c r="P29" s="75"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>510</v>
-      </c>
-      <c r="B30" t="s">
-        <v>510</v>
-      </c>
       <c r="C30" t="s">
         <v>496</v>
       </c>
@@ -6194,28 +6032,28 @@
         <v>145</v>
       </c>
       <c r="E30" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F30" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G30" t="s">
         <v>508</v>
       </c>
       <c r="H30" t="s">
+        <v>511</v>
+      </c>
+      <c r="I30" t="s">
         <v>512</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>513</v>
       </c>
-      <c r="J30" t="s">
-        <v>514</v>
-      </c>
       <c r="K30" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L30" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N30" s="75"/>
       <c r="P30" s="75"/>
@@ -6234,7 +6072,7 @@
         <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F31" t="s">
         <v>11</v>
@@ -6243,19 +6081,19 @@
         <v>509</v>
       </c>
       <c r="H31" t="s">
+        <v>511</v>
+      </c>
+      <c r="I31" t="s">
         <v>512</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>513</v>
       </c>
-      <c r="J31" t="s">
-        <v>514</v>
-      </c>
       <c r="K31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L31" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N31" s="75"/>
       <c r="P31" s="75"/>
@@ -6274,7 +6112,7 @@
         <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
@@ -6283,29 +6121,23 @@
         <v>509</v>
       </c>
       <c r="H32" t="s">
+        <v>511</v>
+      </c>
+      <c r="I32" t="s">
         <v>512</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>513</v>
       </c>
-      <c r="J32" t="s">
-        <v>514</v>
-      </c>
       <c r="K32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L32" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N32" s="75"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>510</v>
-      </c>
-      <c r="B33" t="s">
-        <v>510</v>
-      </c>
       <c r="C33" t="s">
         <v>393</v>
       </c>
@@ -6313,7 +6145,7 @@
         <v>393</v>
       </c>
       <c r="E33" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F33" t="s">
         <v>393</v>
@@ -6322,19 +6154,19 @@
         <v>509</v>
       </c>
       <c r="H33" t="s">
+        <v>511</v>
+      </c>
+      <c r="I33" t="s">
         <v>512</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>513</v>
       </c>
-      <c r="J33" t="s">
-        <v>514</v>
-      </c>
       <c r="K33" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L33" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -6351,7 +6183,7 @@
         <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F34" t="s">
         <v>15</v>
@@ -6360,36 +6192,24 @@
         <v>509</v>
       </c>
       <c r="H34" t="s">
+        <v>511</v>
+      </c>
+      <c r="I34" t="s">
         <v>512</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>513</v>
       </c>
-      <c r="J34" t="s">
-        <v>514</v>
-      </c>
       <c r="K34" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L34" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="E35" t="s">
         <v>510</v>
-      </c>
-      <c r="B35" t="s">
-        <v>510</v>
-      </c>
-      <c r="C35" t="s">
-        <v>510</v>
-      </c>
-      <c r="D35" t="s">
-        <v>510</v>
-      </c>
-      <c r="E35" t="s">
-        <v>511</v>
       </c>
       <c r="F35" t="s">
         <v>15</v>
@@ -6398,28 +6218,22 @@
         <v>509</v>
       </c>
       <c r="H35" t="s">
+        <v>511</v>
+      </c>
+      <c r="I35" t="s">
         <v>512</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>513</v>
       </c>
-      <c r="J35" t="s">
-        <v>514</v>
-      </c>
       <c r="K35" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L35" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>510</v>
-      </c>
-      <c r="B36" t="s">
-        <v>510</v>
-      </c>
       <c r="C36" t="s">
         <v>150</v>
       </c>
@@ -6427,7 +6241,7 @@
         <v>150</v>
       </c>
       <c r="E36" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F36" t="s">
         <v>150</v>
@@ -6436,16 +6250,16 @@
         <v>509</v>
       </c>
       <c r="H36" t="s">
+        <v>511</v>
+      </c>
+      <c r="I36" t="s">
         <v>512</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>513</v>
       </c>
-      <c r="J36" t="s">
-        <v>514</v>
-      </c>
       <c r="K36" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L36" s="75" t="s">
         <v>148</v>
@@ -6454,12 +6268,6 @@
       <c r="P36" s="75"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>510</v>
-      </c>
-      <c r="B37" t="s">
-        <v>510</v>
-      </c>
       <c r="C37" t="s">
         <v>149</v>
       </c>
@@ -6467,7 +6275,7 @@
         <v>149</v>
       </c>
       <c r="E37" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F37" t="s">
         <v>149</v>
@@ -6476,16 +6284,16 @@
         <v>509</v>
       </c>
       <c r="H37" t="s">
+        <v>511</v>
+      </c>
+      <c r="I37" t="s">
         <v>512</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>513</v>
       </c>
-      <c r="J37" t="s">
-        <v>514</v>
-      </c>
       <c r="K37" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L37" s="75" t="s">
         <v>148</v>
@@ -6506,7 +6314,7 @@
         <v>148</v>
       </c>
       <c r="E38" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F38" t="s">
         <v>148</v>
@@ -6515,16 +6323,16 @@
         <v>508</v>
       </c>
       <c r="H38" t="s">
+        <v>511</v>
+      </c>
+      <c r="I38" t="s">
         <v>512</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>513</v>
       </c>
-      <c r="J38" t="s">
-        <v>514</v>
-      </c>
       <c r="K38" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L38" s="75" t="s">
         <v>148</v>
@@ -6535,9 +6343,6 @@
       <c r="A39" t="s">
         <v>34</v>
       </c>
-      <c r="B39" t="s">
-        <v>510</v>
-      </c>
       <c r="C39" t="s">
         <v>153</v>
       </c>
@@ -6545,37 +6350,37 @@
         <v>153</v>
       </c>
       <c r="E39" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F39" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G39" t="s">
         <v>506</v>
       </c>
       <c r="H39" t="s">
+        <v>511</v>
+      </c>
+      <c r="I39" t="s">
         <v>512</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>513</v>
       </c>
-      <c r="J39" t="s">
-        <v>514</v>
-      </c>
       <c r="K39" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L39" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="N39" s="75"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B40" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C40" t="s">
         <v>159</v>
@@ -6584,7 +6389,7 @@
         <v>159</v>
       </c>
       <c r="E40" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F40" t="s">
         <v>7</v>
@@ -6593,19 +6398,19 @@
         <v>509</v>
       </c>
       <c r="H40" t="s">
+        <v>511</v>
+      </c>
+      <c r="I40" t="s">
         <v>512</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>513</v>
       </c>
-      <c r="J40" t="s">
-        <v>514</v>
-      </c>
       <c r="K40" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L40" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N40" s="75"/>
       <c r="P40" s="75"/>
@@ -6617,44 +6422,38 @@
       <c r="B41" t="s">
         <v>37</v>
       </c>
-      <c r="C41" t="s">
-        <v>510</v>
-      </c>
-      <c r="D41" t="s">
-        <v>510</v>
-      </c>
       <c r="E41" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F41" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G41" t="s">
         <v>506</v>
       </c>
       <c r="H41" t="s">
+        <v>511</v>
+      </c>
+      <c r="I41" t="s">
         <v>512</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>513</v>
       </c>
-      <c r="J41" t="s">
-        <v>514</v>
-      </c>
       <c r="K41" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L41" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="P41" s="75"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B42" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C42" t="s">
         <v>158</v>
@@ -6663,37 +6462,37 @@
         <v>158</v>
       </c>
       <c r="E42" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F42" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G42" t="s">
         <v>508</v>
       </c>
       <c r="H42" t="s">
+        <v>511</v>
+      </c>
+      <c r="I42" t="s">
         <v>512</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>513</v>
       </c>
-      <c r="J42" t="s">
-        <v>514</v>
-      </c>
       <c r="K42" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L42" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N42" s="75"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B43" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C43" t="s">
         <v>160</v>
@@ -6702,7 +6501,7 @@
         <v>160</v>
       </c>
       <c r="E43" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F43" t="s">
         <v>147</v>
@@ -6711,36 +6510,27 @@
         <v>508</v>
       </c>
       <c r="H43" t="s">
+        <v>511</v>
+      </c>
+      <c r="I43" t="s">
         <v>512</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>513</v>
       </c>
-      <c r="J43" t="s">
-        <v>514</v>
-      </c>
       <c r="K43" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L43" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>510</v>
-      </c>
-      <c r="B44" t="s">
-        <v>510</v>
-      </c>
       <c r="C44" t="s">
         <v>155</v>
       </c>
-      <c r="D44" t="s">
-        <v>510</v>
-      </c>
       <c r="E44" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F44" t="s">
         <v>142</v>
@@ -6749,16 +6539,16 @@
         <v>508</v>
       </c>
       <c r="H44" t="s">
+        <v>511</v>
+      </c>
+      <c r="I44" t="s">
         <v>512</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>513</v>
       </c>
-      <c r="J44" t="s">
-        <v>514</v>
-      </c>
       <c r="K44" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L44" t="s">
         <v>142</v>
@@ -6771,14 +6561,11 @@
       <c r="B45" t="s">
         <v>41</v>
       </c>
-      <c r="C45" t="s">
-        <v>510</v>
-      </c>
       <c r="D45" t="s">
         <v>155</v>
       </c>
       <c r="E45" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F45" t="s">
         <v>1</v>
@@ -6787,16 +6574,16 @@
         <v>509</v>
       </c>
       <c r="H45" t="s">
+        <v>511</v>
+      </c>
+      <c r="I45" t="s">
         <v>512</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>513</v>
       </c>
-      <c r="J45" t="s">
-        <v>514</v>
-      </c>
       <c r="K45" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L45" t="s">
         <v>142</v>
@@ -6818,68 +6605,59 @@
         <v>154</v>
       </c>
       <c r="E46" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F46" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G46" t="s">
         <v>508</v>
       </c>
       <c r="H46" t="s">
+        <v>511</v>
+      </c>
+      <c r="I46" t="s">
         <v>512</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>513</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
+        <v>513</v>
+      </c>
+      <c r="L46" t="s">
         <v>514</v>
-      </c>
-      <c r="K46" t="s">
-        <v>514</v>
-      </c>
-      <c r="L46" t="s">
-        <v>515</v>
       </c>
       <c r="N46" s="75"/>
       <c r="P46" s="75"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>510</v>
-      </c>
-      <c r="B47" t="s">
-        <v>510</v>
-      </c>
       <c r="C47" t="s">
         <v>156</v>
       </c>
-      <c r="D47" t="s">
-        <v>510</v>
-      </c>
       <c r="E47" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F47" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G47" t="s">
         <v>508</v>
       </c>
       <c r="H47" t="s">
+        <v>511</v>
+      </c>
+      <c r="I47" t="s">
         <v>512</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>513</v>
       </c>
-      <c r="J47" t="s">
-        <v>514</v>
-      </c>
       <c r="K47" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L47" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N47" s="75"/>
       <c r="P47" s="75"/>
@@ -6891,14 +6669,11 @@
       <c r="B48" t="s">
         <v>45</v>
       </c>
-      <c r="C48" t="s">
-        <v>510</v>
-      </c>
       <c r="D48" t="s">
         <v>224</v>
       </c>
       <c r="E48" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F48" t="s">
         <v>5</v>
@@ -6907,19 +6682,19 @@
         <v>507</v>
       </c>
       <c r="H48" t="s">
+        <v>511</v>
+      </c>
+      <c r="I48" t="s">
         <v>512</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>513</v>
       </c>
-      <c r="J48" t="s">
-        <v>514</v>
-      </c>
       <c r="K48" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L48" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P48" s="75"/>
     </row>
@@ -6937,7 +6712,7 @@
         <v>157</v>
       </c>
       <c r="E49" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F49" t="s">
         <v>148</v>
@@ -6946,16 +6721,16 @@
         <v>508</v>
       </c>
       <c r="H49" t="s">
+        <v>511</v>
+      </c>
+      <c r="I49" t="s">
         <v>512</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>513</v>
       </c>
-      <c r="J49" t="s">
-        <v>514</v>
-      </c>
       <c r="K49" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L49" t="s">
         <v>148</v>
@@ -6963,20 +6738,8 @@
       <c r="P49" s="75"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>510</v>
-      </c>
-      <c r="B50" t="s">
-        <v>510</v>
-      </c>
-      <c r="C50" t="s">
-        <v>510</v>
-      </c>
-      <c r="D50" t="s">
-        <v>510</v>
-      </c>
       <c r="E50" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F50" t="s">
         <v>15</v>
@@ -6985,16 +6748,16 @@
         <v>509</v>
       </c>
       <c r="H50" t="s">
+        <v>511</v>
+      </c>
+      <c r="I50" t="s">
         <v>512</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>513</v>
       </c>
-      <c r="J50" t="s">
-        <v>514</v>
-      </c>
       <c r="K50" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L50" t="s">
         <v>147</v>
@@ -7003,20 +6766,8 @@
       <c r="P50" s="75"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>510</v>
-      </c>
-      <c r="B51" t="s">
-        <v>510</v>
-      </c>
-      <c r="C51" t="s">
-        <v>510</v>
-      </c>
-      <c r="D51" t="s">
-        <v>510</v>
-      </c>
       <c r="E51" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F51" t="s">
         <v>11</v>
@@ -7025,29 +6776,23 @@
         <v>509</v>
       </c>
       <c r="H51" t="s">
+        <v>511</v>
+      </c>
+      <c r="I51" t="s">
         <v>512</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>513</v>
       </c>
-      <c r="J51" t="s">
-        <v>514</v>
-      </c>
       <c r="K51" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L51" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N51" s="75"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>510</v>
-      </c>
-      <c r="B52" t="s">
-        <v>510</v>
-      </c>
       <c r="C52" t="s">
         <v>161</v>
       </c>
@@ -7055,46 +6800,40 @@
         <v>161</v>
       </c>
       <c r="E52" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F52" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G52" t="s">
         <v>508</v>
       </c>
       <c r="H52" t="s">
+        <v>511</v>
+      </c>
+      <c r="I52" t="s">
         <v>512</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>513</v>
       </c>
-      <c r="J52" t="s">
-        <v>514</v>
-      </c>
       <c r="K52" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L52" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N52" s="75"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>572</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" t="s">
-        <v>510</v>
-      </c>
-      <c r="D53" t="s">
-        <v>510</v>
+        <v>572</v>
       </c>
       <c r="E53" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F53" t="s">
         <v>7</v>
@@ -7103,27 +6842,27 @@
         <v>509</v>
       </c>
       <c r="H53" t="s">
+        <v>511</v>
+      </c>
+      <c r="I53" t="s">
         <v>512</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>513</v>
       </c>
-      <c r="J53" t="s">
-        <v>514</v>
-      </c>
       <c r="K53" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L53" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>538</v>
+        <v>573</v>
       </c>
       <c r="B54" t="s">
-        <v>538</v>
+        <v>573</v>
       </c>
       <c r="C54" t="s">
         <v>162</v>
@@ -7132,47 +6871,38 @@
         <v>162</v>
       </c>
       <c r="E54" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F54" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G54" t="s">
         <v>508</v>
       </c>
       <c r="H54" t="s">
+        <v>511</v>
+      </c>
+      <c r="I54" t="s">
         <v>512</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>513</v>
       </c>
-      <c r="J54" t="s">
-        <v>514</v>
-      </c>
       <c r="K54" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L54" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N54" s="75"/>
       <c r="P54" s="75"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>510</v>
-      </c>
-      <c r="B55" t="s">
-        <v>510</v>
-      </c>
       <c r="C55" t="s">
         <v>163</v>
       </c>
-      <c r="D55" t="s">
-        <v>510</v>
-      </c>
       <c r="E55" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F55" t="s">
         <v>147</v>
@@ -7181,16 +6911,16 @@
         <v>508</v>
       </c>
       <c r="H55" t="s">
+        <v>511</v>
+      </c>
+      <c r="I55" t="s">
         <v>512</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>513</v>
       </c>
-      <c r="J55" t="s">
-        <v>514</v>
-      </c>
       <c r="K55" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L55" t="s">
         <v>147</v>
@@ -7199,19 +6929,16 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>574</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
-      </c>
-      <c r="C56" t="s">
-        <v>510</v>
+        <v>574</v>
       </c>
       <c r="D56" t="s">
         <v>163</v>
       </c>
       <c r="E56" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F56" t="s">
         <v>15</v>
@@ -7220,16 +6947,16 @@
         <v>509</v>
       </c>
       <c r="H56" t="s">
+        <v>511</v>
+      </c>
+      <c r="I56" t="s">
         <v>512</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>513</v>
       </c>
-      <c r="J56" t="s">
-        <v>514</v>
-      </c>
       <c r="K56" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L56" t="s">
         <v>147</v>
@@ -7237,76 +6964,52 @@
       <c r="N56" s="75"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="E57" t="s">
         <v>510</v>
       </c>
-      <c r="B57" t="s">
-        <v>510</v>
-      </c>
-      <c r="C57" t="s">
-        <v>510</v>
-      </c>
-      <c r="D57" t="s">
-        <v>510</v>
-      </c>
-      <c r="E57" t="s">
-        <v>511</v>
-      </c>
       <c r="F57" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="G57" t="s">
         <v>509</v>
       </c>
       <c r="H57" t="s">
+        <v>511</v>
+      </c>
+      <c r="I57" t="s">
         <v>512</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>513</v>
       </c>
-      <c r="J57" t="s">
-        <v>514</v>
-      </c>
       <c r="K57" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L57" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="E58" t="s">
         <v>510</v>
       </c>
-      <c r="B58" t="s">
-        <v>510</v>
-      </c>
-      <c r="C58" t="s">
-        <v>510</v>
-      </c>
-      <c r="D58" t="s">
-        <v>510</v>
-      </c>
-      <c r="E58" t="s">
-        <v>511</v>
-      </c>
       <c r="F58" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="G58" t="s">
         <v>509</v>
       </c>
       <c r="H58" t="s">
+        <v>511</v>
+      </c>
+      <c r="I58" t="s">
         <v>512</v>
       </c>
-      <c r="I58" t="s">
+      <c r="J58" t="s">
         <v>513</v>
       </c>
-      <c r="J58" t="s">
-        <v>514</v>
-      </c>
       <c r="K58" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L58" t="s">
         <v>151</v>
@@ -7314,38 +7017,26 @@
       <c r="N58" s="75"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="E59" t="s">
         <v>510</v>
       </c>
-      <c r="B59" t="s">
-        <v>510</v>
-      </c>
-      <c r="C59" t="s">
-        <v>510</v>
-      </c>
-      <c r="D59" t="s">
-        <v>510</v>
-      </c>
-      <c r="E59" t="s">
-        <v>511</v>
-      </c>
       <c r="F59" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="G59" t="s">
         <v>509</v>
       </c>
       <c r="H59" t="s">
+        <v>511</v>
+      </c>
+      <c r="I59" t="s">
         <v>512</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>513</v>
       </c>
-      <c r="J59" t="s">
-        <v>514</v>
-      </c>
       <c r="K59" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L59" t="s">
         <v>151</v>
@@ -7354,38 +7045,26 @@
       <c r="P59" s="75"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="E60" t="s">
         <v>510</v>
       </c>
-      <c r="B60" t="s">
-        <v>510</v>
-      </c>
-      <c r="C60" t="s">
-        <v>510</v>
-      </c>
-      <c r="D60" t="s">
-        <v>510</v>
-      </c>
-      <c r="E60" t="s">
-        <v>511</v>
-      </c>
       <c r="F60" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="G60" t="s">
         <v>509</v>
       </c>
       <c r="H60" t="s">
+        <v>511</v>
+      </c>
+      <c r="I60" t="s">
         <v>512</v>
       </c>
-      <c r="I60" t="s">
+      <c r="J60" t="s">
         <v>513</v>
       </c>
-      <c r="J60" t="s">
-        <v>514</v>
-      </c>
       <c r="K60" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L60" t="s">
         <v>151</v>
@@ -7394,114 +7073,78 @@
       <c r="P60" s="75"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="E61" t="s">
         <v>510</v>
       </c>
-      <c r="B61" t="s">
-        <v>510</v>
-      </c>
-      <c r="C61" t="s">
-        <v>510</v>
-      </c>
-      <c r="D61" t="s">
-        <v>510</v>
-      </c>
-      <c r="E61" t="s">
-        <v>511</v>
-      </c>
       <c r="F61" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="G61" t="s">
         <v>509</v>
       </c>
       <c r="H61" t="s">
+        <v>511</v>
+      </c>
+      <c r="I61" t="s">
         <v>512</v>
       </c>
-      <c r="I61" t="s">
+      <c r="J61" t="s">
         <v>513</v>
       </c>
-      <c r="J61" t="s">
-        <v>514</v>
-      </c>
       <c r="K61" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L61" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="E62" t="s">
         <v>510</v>
       </c>
-      <c r="B62" t="s">
-        <v>510</v>
-      </c>
-      <c r="C62" t="s">
-        <v>510</v>
-      </c>
-      <c r="D62" t="s">
-        <v>510</v>
-      </c>
-      <c r="E62" t="s">
-        <v>511</v>
-      </c>
       <c r="F62" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="G62" t="s">
         <v>509</v>
       </c>
       <c r="H62" t="s">
+        <v>511</v>
+      </c>
+      <c r="I62" t="s">
         <v>512</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>513</v>
       </c>
-      <c r="J62" t="s">
-        <v>514</v>
-      </c>
       <c r="K62" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L62" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="E63" t="s">
         <v>510</v>
       </c>
-      <c r="B63" t="s">
-        <v>510</v>
-      </c>
-      <c r="C63" t="s">
-        <v>510</v>
-      </c>
-      <c r="D63" t="s">
-        <v>510</v>
-      </c>
-      <c r="E63" t="s">
-        <v>511</v>
-      </c>
       <c r="F63" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G63" t="s">
         <v>509</v>
       </c>
       <c r="H63" t="s">
+        <v>511</v>
+      </c>
+      <c r="I63" t="s">
         <v>512</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>513</v>
       </c>
-      <c r="J63" t="s">
-        <v>514</v>
-      </c>
       <c r="K63" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L63" t="s">
         <v>151</v>
@@ -7509,10 +7152,10 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>575</v>
       </c>
       <c r="B64" t="s">
-        <v>18</v>
+        <v>575</v>
       </c>
       <c r="C64" t="s">
         <v>131</v>
@@ -7521,7 +7164,7 @@
         <v>131</v>
       </c>
       <c r="E64" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F64" t="s">
         <v>19</v>
@@ -7530,36 +7173,24 @@
         <v>509</v>
       </c>
       <c r="H64" t="s">
+        <v>511</v>
+      </c>
+      <c r="I64" t="s">
         <v>512</v>
       </c>
-      <c r="I64" t="s">
-        <v>513</v>
-      </c>
       <c r="J64" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K64" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L64" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="E65" t="s">
         <v>510</v>
-      </c>
-      <c r="B65" t="s">
-        <v>510</v>
-      </c>
-      <c r="C65" t="s">
-        <v>510</v>
-      </c>
-      <c r="D65" t="s">
-        <v>510</v>
-      </c>
-      <c r="E65" t="s">
-        <v>511</v>
       </c>
       <c r="F65" t="s">
         <v>19</v>
@@ -7568,16 +7199,16 @@
         <v>509</v>
       </c>
       <c r="H65" t="s">
+        <v>511</v>
+      </c>
+      <c r="I65" t="s">
         <v>512</v>
       </c>
-      <c r="I65" t="s">
-        <v>513</v>
-      </c>
       <c r="J65" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K65" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L65" t="s">
         <v>131</v>
@@ -7597,36 +7228,36 @@
         <v>132</v>
       </c>
       <c r="E66" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F66" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G66" t="s">
         <v>508</v>
       </c>
       <c r="H66" t="s">
+        <v>511</v>
+      </c>
+      <c r="I66" t="s">
         <v>512</v>
       </c>
-      <c r="I66" t="s">
-        <v>513</v>
-      </c>
       <c r="J66" t="s">
+        <v>519</v>
+      </c>
+      <c r="K66" t="s">
+        <v>519</v>
+      </c>
+      <c r="L66" t="s">
         <v>520</v>
-      </c>
-      <c r="K66" t="s">
-        <v>520</v>
-      </c>
-      <c r="L66" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B67" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C67" t="s">
         <v>22</v>
@@ -7635,7 +7266,7 @@
         <v>22</v>
       </c>
       <c r="E67" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F67" t="s">
         <v>22</v>
@@ -7644,27 +7275,27 @@
         <v>509</v>
       </c>
       <c r="H67" t="s">
+        <v>511</v>
+      </c>
+      <c r="I67" t="s">
         <v>512</v>
       </c>
-      <c r="I67" t="s">
-        <v>513</v>
-      </c>
       <c r="J67" t="s">
+        <v>519</v>
+      </c>
+      <c r="K67" t="s">
+        <v>519</v>
+      </c>
+      <c r="L67" t="s">
         <v>520</v>
-      </c>
-      <c r="K67" t="s">
-        <v>520</v>
-      </c>
-      <c r="L67" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B68" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C68" t="s">
         <v>23</v>
@@ -7673,7 +7304,7 @@
         <v>23</v>
       </c>
       <c r="E68" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F68" t="s">
         <v>23</v>
@@ -7682,19 +7313,19 @@
         <v>509</v>
       </c>
       <c r="H68" t="s">
+        <v>511</v>
+      </c>
+      <c r="I68" t="s">
         <v>512</v>
       </c>
-      <c r="I68" t="s">
-        <v>513</v>
-      </c>
       <c r="J68" t="s">
+        <v>519</v>
+      </c>
+      <c r="K68" t="s">
+        <v>519</v>
+      </c>
+      <c r="L68" t="s">
         <v>520</v>
-      </c>
-      <c r="K68" t="s">
-        <v>520</v>
-      </c>
-      <c r="L68" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -7711,7 +7342,7 @@
         <v>25</v>
       </c>
       <c r="E69" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F69" t="s">
         <v>25</v>
@@ -7720,19 +7351,19 @@
         <v>509</v>
       </c>
       <c r="H69" t="s">
+        <v>511</v>
+      </c>
+      <c r="I69" t="s">
         <v>512</v>
       </c>
-      <c r="I69" t="s">
-        <v>513</v>
-      </c>
       <c r="J69" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K69" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L69" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -7749,7 +7380,7 @@
         <v>27</v>
       </c>
       <c r="E70" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F70" t="s">
         <v>27</v>
@@ -7758,28 +7389,25 @@
         <v>509</v>
       </c>
       <c r="H70" t="s">
+        <v>511</v>
+      </c>
+      <c r="I70" t="s">
         <v>512</v>
       </c>
-      <c r="I70" t="s">
-        <v>513</v>
-      </c>
       <c r="J70" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K70" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L70" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
-      <c r="B71" t="s">
-        <v>510</v>
-      </c>
       <c r="C71" t="s">
         <v>495</v>
       </c>
@@ -7787,63 +7415,57 @@
         <v>133</v>
       </c>
       <c r="E71" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F71" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G71" t="s">
         <v>508</v>
       </c>
       <c r="H71" t="s">
+        <v>511</v>
+      </c>
+      <c r="I71" t="s">
         <v>512</v>
       </c>
-      <c r="I71" t="s">
-        <v>513</v>
-      </c>
       <c r="J71" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K71" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L71" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
         <v>524</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>510</v>
-      </c>
-      <c r="B72" t="s">
-        <v>510</v>
-      </c>
-      <c r="C72" t="s">
-        <v>525</v>
       </c>
       <c r="D72" t="s">
         <v>134</v>
       </c>
       <c r="E72" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F72" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G72" t="s">
         <v>506</v>
       </c>
       <c r="H72" t="s">
+        <v>511</v>
+      </c>
+      <c r="I72" t="s">
         <v>512</v>
       </c>
-      <c r="I72" t="s">
-        <v>513</v>
-      </c>
       <c r="J72" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K72" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L72" t="s">
         <v>135</v>
@@ -7863,63 +7485,54 @@
         <v>135</v>
       </c>
       <c r="E73" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F73" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G73" t="s">
         <v>506</v>
       </c>
       <c r="H73" t="s">
+        <v>511</v>
+      </c>
+      <c r="I73" t="s">
         <v>512</v>
       </c>
-      <c r="I73" t="s">
-        <v>513</v>
-      </c>
       <c r="J73" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K73" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L73" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>510</v>
-      </c>
-      <c r="B74" t="s">
-        <v>510</v>
-      </c>
-      <c r="C74" t="s">
-        <v>510</v>
-      </c>
       <c r="D74" t="s">
         <v>311</v>
       </c>
       <c r="E74" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F74" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G74" t="s">
         <v>506</v>
       </c>
       <c r="H74" t="s">
+        <v>511</v>
+      </c>
+      <c r="I74" t="s">
         <v>512</v>
       </c>
-      <c r="I74" t="s">
-        <v>513</v>
-      </c>
       <c r="J74" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K74" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L74" t="s">
         <v>135</v>
@@ -7929,9 +7542,6 @@
       <c r="A75" t="s">
         <v>49</v>
       </c>
-      <c r="B75" t="s">
-        <v>510</v>
-      </c>
       <c r="C75" t="s">
         <v>477</v>
       </c>
@@ -7939,25 +7549,25 @@
         <v>112</v>
       </c>
       <c r="E75" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F75" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G75" t="s">
         <v>506</v>
       </c>
       <c r="H75" t="s">
+        <v>511</v>
+      </c>
+      <c r="I75" t="s">
         <v>512</v>
       </c>
-      <c r="I75" t="s">
-        <v>513</v>
-      </c>
       <c r="J75" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K75" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L75" t="s">
         <v>135</v>
@@ -7965,133 +7575,109 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B76" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C76" t="s">
         <v>165</v>
       </c>
-      <c r="D76" t="s">
-        <v>510</v>
-      </c>
       <c r="E76" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F76" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G76" t="s">
         <v>508</v>
       </c>
       <c r="H76" t="s">
+        <v>511</v>
+      </c>
+      <c r="I76" t="s">
         <v>512</v>
       </c>
-      <c r="I76" t="s">
-        <v>513</v>
-      </c>
       <c r="J76" t="s">
+        <v>519</v>
+      </c>
+      <c r="K76" t="s">
+        <v>519</v>
+      </c>
+      <c r="L76" t="s">
         <v>520</v>
-      </c>
-      <c r="K76" t="s">
-        <v>520</v>
-      </c>
-      <c r="L76" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B77" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C77" t="s">
         <v>166</v>
       </c>
-      <c r="D77" t="s">
-        <v>510</v>
-      </c>
       <c r="E77" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F77" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G77" t="s">
         <v>508</v>
       </c>
       <c r="H77" t="s">
+        <v>511</v>
+      </c>
+      <c r="I77" t="s">
         <v>512</v>
       </c>
-      <c r="I77" t="s">
-        <v>513</v>
-      </c>
       <c r="J77" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K77" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L77" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B78" t="s">
-        <v>534</v>
-      </c>
-      <c r="C78" t="s">
-        <v>510</v>
-      </c>
-      <c r="D78" t="s">
-        <v>510</v>
+        <v>533</v>
       </c>
       <c r="E78" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F78" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G78" t="s">
         <v>506</v>
       </c>
       <c r="H78" t="s">
+        <v>511</v>
+      </c>
+      <c r="I78" t="s">
         <v>512</v>
       </c>
-      <c r="I78" t="s">
-        <v>513</v>
-      </c>
       <c r="J78" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K78" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L78" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>510</v>
-      </c>
-      <c r="B79" t="s">
-        <v>510</v>
-      </c>
-      <c r="C79" t="s">
-        <v>510</v>
-      </c>
-      <c r="D79" t="s">
-        <v>510</v>
-      </c>
       <c r="E79" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F79" t="s">
         <v>19</v>
@@ -8100,36 +7686,27 @@
         <v>509</v>
       </c>
       <c r="H79" t="s">
+        <v>511</v>
+      </c>
+      <c r="I79" t="s">
         <v>512</v>
       </c>
-      <c r="I79" t="s">
-        <v>513</v>
-      </c>
       <c r="J79" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K79" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L79" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>510</v>
-      </c>
-      <c r="B80" t="s">
-        <v>510</v>
-      </c>
-      <c r="C80" t="s">
-        <v>510</v>
-      </c>
       <c r="D80" t="s">
         <v>261</v>
       </c>
       <c r="E80" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F80" t="s">
         <v>261</v>
@@ -8138,36 +7715,27 @@
         <v>508</v>
       </c>
       <c r="H80" t="s">
+        <v>511</v>
+      </c>
+      <c r="I80" t="s">
         <v>512</v>
       </c>
-      <c r="I80" t="s">
-        <v>513</v>
-      </c>
       <c r="J80" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K80" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L80" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>510</v>
-      </c>
-      <c r="B81" t="s">
-        <v>510</v>
-      </c>
-      <c r="C81" t="s">
-        <v>510</v>
-      </c>
+    <row r="81" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
         <v>230</v>
       </c>
       <c r="E81" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F81" t="s">
         <v>230</v>
@@ -8176,36 +7744,27 @@
         <v>508</v>
       </c>
       <c r="H81" t="s">
+        <v>511</v>
+      </c>
+      <c r="I81" t="s">
         <v>512</v>
       </c>
-      <c r="I81" t="s">
-        <v>513</v>
-      </c>
       <c r="J81" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K81" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L81" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>510</v>
-      </c>
-      <c r="B82" t="s">
-        <v>510</v>
-      </c>
-      <c r="C82" t="s">
-        <v>510</v>
-      </c>
+    <row r="82" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
         <v>237</v>
       </c>
       <c r="E82" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F82" t="s">
         <v>237</v>
@@ -8214,606 +7773,420 @@
         <v>508</v>
       </c>
       <c r="H82" t="s">
+        <v>511</v>
+      </c>
+      <c r="I82" t="s">
         <v>512</v>
       </c>
-      <c r="I82" t="s">
-        <v>513</v>
-      </c>
       <c r="J82" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K82" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L82" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>510</v>
-      </c>
-      <c r="B83" t="s">
-        <v>510</v>
-      </c>
-      <c r="C83" t="s">
-        <v>510</v>
-      </c>
+    <row r="83" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
         <v>223</v>
       </c>
       <c r="E83" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F83" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G83" t="s">
         <v>509</v>
       </c>
       <c r="H83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I83" t="s">
         <v>512</v>
       </c>
-      <c r="I83" t="s">
-        <v>513</v>
-      </c>
       <c r="J83" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K83" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L83" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="84" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
         <v>510</v>
       </c>
-      <c r="B84" t="s">
-        <v>510</v>
-      </c>
-      <c r="C84" t="s">
-        <v>510</v>
-      </c>
-      <c r="D84" t="s">
-        <v>510</v>
-      </c>
-      <c r="E84" t="s">
-        <v>511</v>
-      </c>
       <c r="F84" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="G84" t="s">
         <v>509</v>
       </c>
       <c r="H84" t="s">
+        <v>511</v>
+      </c>
+      <c r="I84" t="s">
         <v>512</v>
       </c>
-      <c r="I84" t="s">
-        <v>513</v>
-      </c>
       <c r="J84" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K84" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L84" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="85" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
         <v>510</v>
       </c>
-      <c r="B85" t="s">
-        <v>510</v>
-      </c>
-      <c r="C85" t="s">
-        <v>510</v>
-      </c>
-      <c r="D85" t="s">
-        <v>510</v>
-      </c>
-      <c r="E85" t="s">
-        <v>511</v>
-      </c>
       <c r="F85" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="G85" t="s">
         <v>509</v>
       </c>
       <c r="H85" t="s">
+        <v>511</v>
+      </c>
+      <c r="I85" t="s">
         <v>512</v>
       </c>
-      <c r="I85" t="s">
-        <v>513</v>
-      </c>
       <c r="J85" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K85" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L85" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="86" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
         <v>510</v>
       </c>
-      <c r="B86" t="s">
-        <v>510</v>
-      </c>
-      <c r="C86" t="s">
-        <v>510</v>
-      </c>
-      <c r="D86" t="s">
-        <v>510</v>
-      </c>
-      <c r="E86" t="s">
-        <v>511</v>
-      </c>
       <c r="F86" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="G86" t="s">
         <v>509</v>
       </c>
       <c r="H86" t="s">
+        <v>511</v>
+      </c>
+      <c r="I86" t="s">
         <v>512</v>
       </c>
-      <c r="I86" t="s">
-        <v>513</v>
-      </c>
       <c r="J86" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K86" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L86" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="87" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
         <v>510</v>
       </c>
-      <c r="B87" t="s">
-        <v>510</v>
-      </c>
-      <c r="C87" t="s">
-        <v>510</v>
-      </c>
-      <c r="D87" t="s">
-        <v>510</v>
-      </c>
-      <c r="E87" t="s">
-        <v>511</v>
-      </c>
       <c r="F87" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="G87" t="s">
         <v>509</v>
       </c>
       <c r="H87" t="s">
+        <v>511</v>
+      </c>
+      <c r="I87" t="s">
         <v>512</v>
       </c>
-      <c r="I87" t="s">
-        <v>513</v>
-      </c>
       <c r="J87" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K87" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L87" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="88" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
         <v>510</v>
       </c>
-      <c r="B88" t="s">
-        <v>510</v>
-      </c>
-      <c r="C88" t="s">
-        <v>510</v>
-      </c>
-      <c r="D88" t="s">
-        <v>510</v>
-      </c>
-      <c r="E88" t="s">
-        <v>511</v>
-      </c>
       <c r="F88" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="G88" t="s">
         <v>509</v>
       </c>
       <c r="H88" t="s">
+        <v>511</v>
+      </c>
+      <c r="I88" t="s">
         <v>512</v>
       </c>
-      <c r="I88" t="s">
-        <v>513</v>
-      </c>
       <c r="J88" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K88" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L88" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="89" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
         <v>510</v>
       </c>
-      <c r="B89" t="s">
-        <v>510</v>
-      </c>
-      <c r="C89" t="s">
-        <v>510</v>
-      </c>
-      <c r="D89" t="s">
-        <v>510</v>
-      </c>
-      <c r="E89" t="s">
-        <v>511</v>
-      </c>
       <c r="F89" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="G89" t="s">
         <v>509</v>
       </c>
       <c r="H89" t="s">
+        <v>511</v>
+      </c>
+      <c r="I89" t="s">
         <v>512</v>
       </c>
-      <c r="I89" t="s">
-        <v>513</v>
-      </c>
       <c r="J89" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K89" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L89" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>510</v>
-      </c>
-      <c r="B90" t="s">
-        <v>510</v>
-      </c>
-      <c r="C90" t="s">
-        <v>510</v>
-      </c>
-      <c r="D90" t="s">
-        <v>510</v>
-      </c>
+    <row r="90" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E90" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F90" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="G90" t="s">
         <v>509</v>
       </c>
       <c r="H90" t="s">
+        <v>511</v>
+      </c>
+      <c r="I90" t="s">
         <v>512</v>
       </c>
-      <c r="I90" t="s">
-        <v>513</v>
-      </c>
       <c r="J90" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K90" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L90" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="91" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
         <v>510</v>
       </c>
-      <c r="B91" t="s">
-        <v>510</v>
-      </c>
-      <c r="C91" t="s">
-        <v>510</v>
-      </c>
-      <c r="D91" t="s">
-        <v>510</v>
-      </c>
-      <c r="E91" t="s">
-        <v>511</v>
-      </c>
       <c r="F91" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="G91" t="s">
         <v>509</v>
       </c>
       <c r="H91" t="s">
+        <v>511</v>
+      </c>
+      <c r="I91" t="s">
         <v>512</v>
       </c>
-      <c r="I91" t="s">
-        <v>513</v>
-      </c>
       <c r="J91" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K91" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L91" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="92" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
         <v>510</v>
       </c>
-      <c r="B92" t="s">
-        <v>510</v>
-      </c>
-      <c r="C92" t="s">
-        <v>510</v>
-      </c>
-      <c r="D92" t="s">
-        <v>510</v>
-      </c>
-      <c r="E92" t="s">
-        <v>511</v>
-      </c>
       <c r="F92" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="G92" t="s">
         <v>509</v>
       </c>
       <c r="H92" t="s">
+        <v>511</v>
+      </c>
+      <c r="I92" t="s">
         <v>512</v>
       </c>
-      <c r="I92" t="s">
-        <v>513</v>
-      </c>
       <c r="J92" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K92" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L92" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="93" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
         <v>510</v>
       </c>
-      <c r="B93" t="s">
-        <v>510</v>
-      </c>
-      <c r="C93" t="s">
-        <v>510</v>
-      </c>
-      <c r="D93" t="s">
-        <v>510</v>
-      </c>
-      <c r="E93" t="s">
-        <v>511</v>
-      </c>
       <c r="F93" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="G93" t="s">
         <v>509</v>
       </c>
       <c r="H93" t="s">
+        <v>511</v>
+      </c>
+      <c r="I93" t="s">
         <v>512</v>
       </c>
-      <c r="I93" t="s">
-        <v>513</v>
-      </c>
       <c r="J93" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K93" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L93" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="94" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
         <v>510</v>
       </c>
-      <c r="B94" t="s">
-        <v>510</v>
-      </c>
-      <c r="C94" t="s">
-        <v>510</v>
-      </c>
-      <c r="D94" t="s">
-        <v>510</v>
-      </c>
-      <c r="E94" t="s">
-        <v>511</v>
-      </c>
       <c r="F94" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="G94" t="s">
         <v>509</v>
       </c>
       <c r="H94" t="s">
+        <v>511</v>
+      </c>
+      <c r="I94" t="s">
         <v>512</v>
       </c>
-      <c r="I94" t="s">
-        <v>513</v>
-      </c>
       <c r="J94" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K94" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L94" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="95" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
         <v>510</v>
       </c>
-      <c r="B95" t="s">
-        <v>510</v>
-      </c>
-      <c r="C95" t="s">
-        <v>510</v>
-      </c>
-      <c r="D95" t="s">
-        <v>510</v>
-      </c>
-      <c r="E95" t="s">
-        <v>511</v>
-      </c>
       <c r="F95" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="G95" t="s">
         <v>509</v>
       </c>
       <c r="H95" t="s">
+        <v>511</v>
+      </c>
+      <c r="I95" t="s">
         <v>512</v>
       </c>
-      <c r="I95" t="s">
-        <v>513</v>
-      </c>
       <c r="J95" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K95" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L95" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="96" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
         <v>510</v>
       </c>
-      <c r="B96" t="s">
-        <v>510</v>
-      </c>
-      <c r="C96" t="s">
-        <v>510</v>
-      </c>
-      <c r="D96" t="s">
-        <v>510</v>
-      </c>
-      <c r="E96" t="s">
-        <v>511</v>
-      </c>
       <c r="F96" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="G96" t="s">
         <v>509</v>
       </c>
       <c r="H96" t="s">
+        <v>511</v>
+      </c>
+      <c r="I96" t="s">
         <v>512</v>
       </c>
-      <c r="I96" t="s">
-        <v>513</v>
-      </c>
       <c r="J96" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K96" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L96" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="E97" t="s">
         <v>510</v>
       </c>
-      <c r="B97" t="s">
-        <v>510</v>
-      </c>
-      <c r="C97" t="s">
-        <v>510</v>
-      </c>
-      <c r="D97" t="s">
-        <v>510</v>
-      </c>
-      <c r="E97" t="s">
-        <v>511</v>
-      </c>
       <c r="F97" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="G97" t="s">
         <v>509</v>
       </c>
       <c r="H97" t="s">
+        <v>511</v>
+      </c>
+      <c r="I97" t="s">
         <v>512</v>
       </c>
-      <c r="I97" t="s">
-        <v>513</v>
-      </c>
       <c r="J97" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K97" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L97" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>510</v>
-      </c>
-      <c r="B98" t="s">
-        <v>510</v>
-      </c>
-      <c r="C98" t="s">
-        <v>510</v>
-      </c>
       <c r="D98" t="s">
         <v>363</v>
       </c>
       <c r="E98" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F98" t="s">
         <v>363</v>
@@ -8822,36 +8195,27 @@
         <v>508</v>
       </c>
       <c r="H98" t="s">
+        <v>511</v>
+      </c>
+      <c r="I98" t="s">
         <v>512</v>
       </c>
-      <c r="I98" t="s">
-        <v>513</v>
-      </c>
       <c r="J98" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K98" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L98" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>510</v>
-      </c>
-      <c r="B99" t="s">
-        <v>510</v>
-      </c>
-      <c r="C99" t="s">
-        <v>510</v>
-      </c>
       <c r="D99" t="s">
         <v>340</v>
       </c>
       <c r="E99" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F99" t="s">
         <v>340</v>
@@ -8860,36 +8224,27 @@
         <v>508</v>
       </c>
       <c r="H99" t="s">
+        <v>511</v>
+      </c>
+      <c r="I99" t="s">
         <v>512</v>
       </c>
-      <c r="I99" t="s">
-        <v>513</v>
-      </c>
       <c r="J99" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K99" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L99" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>510</v>
-      </c>
-      <c r="B100" t="s">
-        <v>510</v>
-      </c>
-      <c r="C100" t="s">
-        <v>510</v>
-      </c>
       <c r="D100" t="s">
         <v>368</v>
       </c>
       <c r="E100" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F100" t="s">
         <v>368</v>
@@ -8898,16 +8253,16 @@
         <v>508</v>
       </c>
       <c r="H100" t="s">
+        <v>511</v>
+      </c>
+      <c r="I100" t="s">
         <v>512</v>
       </c>
-      <c r="I100" t="s">
-        <v>513</v>
-      </c>
       <c r="J100" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K100" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L100" t="s">
         <v>368</v>
@@ -8927,186 +8282,144 @@
         <v>164</v>
       </c>
       <c r="E101" t="s">
+        <v>525</v>
+      </c>
+      <c r="F101" t="s">
         <v>526</v>
-      </c>
-      <c r="F101" t="s">
-        <v>527</v>
       </c>
       <c r="G101" t="s">
         <v>506</v>
       </c>
       <c r="H101" t="s">
+        <v>511</v>
+      </c>
+      <c r="I101" t="s">
         <v>512</v>
       </c>
-      <c r="I101" t="s">
-        <v>513</v>
-      </c>
       <c r="J101" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="K101" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="L101" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>54</v>
-      </c>
-      <c r="B102" t="s">
-        <v>510</v>
+        <v>576</v>
       </c>
       <c r="C102" t="s">
         <v>476</v>
       </c>
-      <c r="D102" t="s">
-        <v>510</v>
-      </c>
       <c r="E102" t="s">
+        <v>534</v>
+      </c>
+      <c r="F102" t="s">
+        <v>512</v>
+      </c>
+      <c r="G102" t="s">
         <v>535</v>
       </c>
-      <c r="F102" t="s">
-        <v>513</v>
-      </c>
-      <c r="G102" t="s">
-        <v>536</v>
-      </c>
       <c r="H102" t="s">
+        <v>511</v>
+      </c>
+      <c r="I102" t="s">
         <v>512</v>
       </c>
-      <c r="I102" t="s">
-        <v>513</v>
-      </c>
-      <c r="J102" t="s">
-        <v>510</v>
-      </c>
       <c r="K102" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L102" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>537</v>
+        <v>577</v>
       </c>
       <c r="B103" t="s">
-        <v>537</v>
-      </c>
-      <c r="C103" t="s">
-        <v>510</v>
+        <v>577</v>
       </c>
       <c r="D103" t="s">
         <v>129</v>
       </c>
       <c r="E103" t="s">
+        <v>534</v>
+      </c>
+      <c r="F103" t="s">
+        <v>512</v>
+      </c>
+      <c r="G103" t="s">
         <v>535</v>
       </c>
-      <c r="F103" t="s">
-        <v>513</v>
-      </c>
-      <c r="G103" t="s">
-        <v>536</v>
-      </c>
       <c r="H103" t="s">
+        <v>511</v>
+      </c>
+      <c r="I103" t="s">
         <v>512</v>
       </c>
-      <c r="I103" t="s">
-        <v>513</v>
-      </c>
-      <c r="J103" t="s">
-        <v>510</v>
-      </c>
       <c r="K103" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L103" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>510</v>
-      </c>
-      <c r="B104" t="s">
-        <v>510</v>
-      </c>
-      <c r="C104" t="s">
-        <v>510</v>
-      </c>
       <c r="D104" t="s">
         <v>198</v>
       </c>
       <c r="E104" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F104" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G104" t="s">
         <v>505</v>
       </c>
       <c r="H104" t="s">
+        <v>511</v>
+      </c>
+      <c r="I104" t="s">
         <v>512</v>
       </c>
-      <c r="I104" t="s">
-        <v>513</v>
-      </c>
-      <c r="J104" t="s">
-        <v>510</v>
-      </c>
       <c r="K104" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L104" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>510</v>
-      </c>
-      <c r="B105" t="s">
-        <v>510</v>
-      </c>
-      <c r="C105" t="s">
-        <v>510</v>
-      </c>
       <c r="D105" t="s">
         <v>262</v>
       </c>
       <c r="E105" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F105" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G105" t="s">
         <v>505</v>
       </c>
       <c r="H105" t="s">
+        <v>511</v>
+      </c>
+      <c r="I105" t="s">
         <v>512</v>
       </c>
-      <c r="I105" t="s">
-        <v>513</v>
-      </c>
-      <c r="J105" t="s">
-        <v>510</v>
-      </c>
       <c r="K105" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L105" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>510</v>
-      </c>
       <c r="B106" t="s">
         <v>178</v>
       </c>
@@ -9117,28 +8430,28 @@
         <v>179</v>
       </c>
       <c r="E106" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F106" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="G106" t="s">
         <v>506</v>
       </c>
       <c r="H106" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I106" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="J106" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="K106" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="L106" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -9155,36 +8468,36 @@
         <v>173</v>
       </c>
       <c r="E107" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F107" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="G107" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="H107" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I107" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="J107" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="K107" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="L107" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>84</v>
+        <v>578</v>
       </c>
       <c r="B108" t="s">
-        <v>84</v>
+        <v>578</v>
       </c>
       <c r="C108" t="s">
         <v>480</v>
@@ -9193,22 +8506,19 @@
         <v>128</v>
       </c>
       <c r="E108" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F108" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="G108" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="H108" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="I108" t="s">
-        <v>543</v>
-      </c>
-      <c r="J108" t="s">
-        <v>510</v>
+        <v>540</v>
       </c>
       <c r="K108" t="s">
         <v>128</v>
@@ -9231,7 +8541,7 @@
         <v>167</v>
       </c>
       <c r="E109" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F109" t="s">
         <v>167</v>
@@ -9240,19 +8550,19 @@
         <v>508</v>
       </c>
       <c r="H109" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I109" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J109" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="K109" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L109" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
@@ -9269,7 +8579,7 @@
         <v>168</v>
       </c>
       <c r="E110" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F110" t="s">
         <v>168</v>
@@ -9278,19 +8588,19 @@
         <v>508</v>
       </c>
       <c r="H110" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I110" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J110" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="K110" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L110" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
@@ -9307,7 +8617,7 @@
         <v>169</v>
       </c>
       <c r="E111" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F111" t="s">
         <v>169</v>
@@ -9316,19 +8626,19 @@
         <v>508</v>
       </c>
       <c r="H111" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I111" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J111" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="K111" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L111" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
@@ -9345,7 +8655,7 @@
         <v>170</v>
       </c>
       <c r="E112" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F112" t="s">
         <v>170</v>
@@ -9354,28 +8664,25 @@
         <v>508</v>
       </c>
       <c r="H112" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I112" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J112" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="K112" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L112" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>80</v>
       </c>
-      <c r="B113" t="s">
-        <v>510</v>
-      </c>
       <c r="C113" t="s">
         <v>81</v>
       </c>
@@ -9383,7 +8690,7 @@
         <v>81</v>
       </c>
       <c r="E113" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F113" t="s">
         <v>81</v>
@@ -9392,19 +8699,19 @@
         <v>509</v>
       </c>
       <c r="H113" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I113" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J113" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="K113" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L113" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
@@ -9421,7 +8728,7 @@
         <v>174</v>
       </c>
       <c r="E114" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F114" t="s">
         <v>174</v>
@@ -9430,36 +8737,27 @@
         <v>508</v>
       </c>
       <c r="H114" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I114" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J114" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="K114" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L114" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>510</v>
-      </c>
-      <c r="B115" t="s">
-        <v>510</v>
-      </c>
-      <c r="C115" t="s">
-        <v>510</v>
-      </c>
       <c r="D115" t="s">
         <v>264</v>
       </c>
       <c r="E115" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F115" t="s">
         <v>264</v>
@@ -9468,36 +8766,27 @@
         <v>508</v>
       </c>
       <c r="H115" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I115" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J115" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="K115" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L115" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>510</v>
-      </c>
-      <c r="B116" t="s">
-        <v>510</v>
-      </c>
-      <c r="C116" t="s">
-        <v>510</v>
-      </c>
       <c r="D116" t="s">
         <v>249</v>
       </c>
       <c r="E116" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F116" t="s">
         <v>249</v>
@@ -9506,36 +8795,27 @@
         <v>508</v>
       </c>
       <c r="H116" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I116" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J116" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="K116" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L116" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>510</v>
-      </c>
-      <c r="B117" t="s">
-        <v>510</v>
-      </c>
-      <c r="C117" t="s">
-        <v>510</v>
-      </c>
       <c r="D117" t="s">
         <v>211</v>
       </c>
       <c r="E117" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F117" t="s">
         <v>211</v>
@@ -9544,57 +8824,42 @@
         <v>508</v>
       </c>
       <c r="H117" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I117" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J117" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="K117" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L117" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>510</v>
-      </c>
-      <c r="B118" t="s">
-        <v>510</v>
-      </c>
       <c r="C118" t="s">
         <v>484</v>
       </c>
-      <c r="D118" t="s">
+      <c r="E118" t="s">
         <v>510</v>
       </c>
-      <c r="E118" t="s">
-        <v>511</v>
-      </c>
       <c r="F118" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G118" t="s">
         <v>504</v>
       </c>
       <c r="H118" t="s">
-        <v>540</v>
-      </c>
-      <c r="I118" t="s">
-        <v>510</v>
-      </c>
-      <c r="J118" t="s">
-        <v>510</v>
+        <v>537</v>
       </c>
       <c r="K118" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L118" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
@@ -9611,28 +8876,22 @@
         <v>171</v>
       </c>
       <c r="E119" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F119" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G119" t="s">
         <v>504</v>
       </c>
       <c r="H119" t="s">
-        <v>540</v>
-      </c>
-      <c r="I119" t="s">
-        <v>510</v>
-      </c>
-      <c r="J119" t="s">
-        <v>510</v>
+        <v>537</v>
       </c>
       <c r="K119" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L119" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further analysis of zooplankton bliz
</commit_message>
<xml_diff>
--- a/FRP_EMPcrosswalk.xlsx
+++ b/FRP_EMPcrosswalk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/ZoopAnalyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="11_D1D8BACF3E4A32804D628C8F00905AC72DA55AA6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{65A613F8-C2D1-44DC-B2B6-1FACEE1CF9DB}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="11_D1D8BACF3E4A32804D628C8F00905AC72DA55AA6" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E87CB816-5865-47DC-9630-A00451583A17}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3023" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="578">
   <si>
     <t>ACARTELA</t>
   </si>
@@ -1930,9 +1930,6 @@
   </si>
   <si>
     <t>Malacostraca</t>
-  </si>
-  <si>
-    <t>Cumacea</t>
   </si>
   <si>
     <t>Latona</t>
@@ -5032,16 +5029,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BB1C86-82F6-4832-A5D9-91E8E1316434}">
-  <dimension ref="A1:R119"/>
+  <dimension ref="A1:R118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A106" sqref="A106:XFD106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="23.140625" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
@@ -5084,7 +5081,7 @@
         <v>422</v>
       </c>
       <c r="L1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -5117,10 +5114,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C3" t="s">
         <v>136</v>
@@ -5373,13 +5370,13 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E10" t="s">
         <v>510</v>
       </c>
       <c r="F10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G10" t="s">
         <v>508</v>
@@ -5650,7 +5647,7 @@
         <v>510</v>
       </c>
       <c r="F19" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G19" t="s">
         <v>509</v>
@@ -5678,7 +5675,7 @@
         <v>510</v>
       </c>
       <c r="F20" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G20" t="s">
         <v>509</v>
@@ -5916,7 +5913,7 @@
         <v>513</v>
       </c>
       <c r="L26" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="P26" s="75"/>
     </row>
@@ -6069,7 +6066,7 @@
         <v>146</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="E31" t="s">
         <v>510</v>
@@ -6827,10 +6824,10 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B53" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E53" t="s">
         <v>534</v>
@@ -6859,10 +6856,10 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B54" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C54" t="s">
         <v>162</v>
@@ -6929,10 +6926,10 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B56" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D56" t="s">
         <v>163</v>
@@ -6968,7 +6965,7 @@
         <v>510</v>
       </c>
       <c r="F57" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G57" t="s">
         <v>509</v>
@@ -6994,7 +6991,7 @@
         <v>510</v>
       </c>
       <c r="F58" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G58" t="s">
         <v>509</v>
@@ -7021,7 +7018,7 @@
         <v>510</v>
       </c>
       <c r="F59" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G59" t="s">
         <v>509</v>
@@ -7049,7 +7046,7 @@
         <v>510</v>
       </c>
       <c r="F60" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G60" t="s">
         <v>509</v>
@@ -7077,7 +7074,7 @@
         <v>510</v>
       </c>
       <c r="F61" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G61" t="s">
         <v>509</v>
@@ -7103,7 +7100,7 @@
         <v>510</v>
       </c>
       <c r="F62" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G62" t="s">
         <v>509</v>
@@ -7129,7 +7126,7 @@
         <v>510</v>
       </c>
       <c r="F63" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G63" t="s">
         <v>509</v>
@@ -7152,10 +7149,10 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B64" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C64" t="s">
         <v>131</v>
@@ -7727,7 +7724,7 @@
         <v>519</v>
       </c>
       <c r="L80" t="s">
-        <v>261</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="4:12" x14ac:dyDescent="0.25">
@@ -7756,7 +7753,7 @@
         <v>519</v>
       </c>
       <c r="L81" t="s">
-        <v>230</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="4:12" x14ac:dyDescent="0.25">
@@ -7785,7 +7782,7 @@
         <v>519</v>
       </c>
       <c r="L82" t="s">
-        <v>237</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" spans="4:12" x14ac:dyDescent="0.25">
@@ -7796,7 +7793,7 @@
         <v>510</v>
       </c>
       <c r="F83" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G83" t="s">
         <v>509</v>
@@ -7814,7 +7811,7 @@
         <v>519</v>
       </c>
       <c r="L83" t="s">
-        <v>223</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="4:12" x14ac:dyDescent="0.25">
@@ -7822,7 +7819,7 @@
         <v>510</v>
       </c>
       <c r="F84" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G84" t="s">
         <v>509</v>
@@ -7848,7 +7845,7 @@
         <v>510</v>
       </c>
       <c r="F85" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G85" t="s">
         <v>509</v>
@@ -7874,7 +7871,7 @@
         <v>510</v>
       </c>
       <c r="F86" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G86" t="s">
         <v>509</v>
@@ -7900,7 +7897,7 @@
         <v>510</v>
       </c>
       <c r="F87" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G87" t="s">
         <v>509</v>
@@ -7926,7 +7923,7 @@
         <v>510</v>
       </c>
       <c r="F88" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G88" t="s">
         <v>509</v>
@@ -7952,7 +7949,7 @@
         <v>510</v>
       </c>
       <c r="F89" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G89" t="s">
         <v>509</v>
@@ -7978,7 +7975,7 @@
         <v>527</v>
       </c>
       <c r="F90" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G90" t="s">
         <v>509</v>
@@ -8004,7 +8001,7 @@
         <v>510</v>
       </c>
       <c r="F91" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G91" t="s">
         <v>509</v>
@@ -8030,7 +8027,7 @@
         <v>510</v>
       </c>
       <c r="F92" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G92" t="s">
         <v>509</v>
@@ -8056,7 +8053,7 @@
         <v>510</v>
       </c>
       <c r="F93" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G93" t="s">
         <v>509</v>
@@ -8082,7 +8079,7 @@
         <v>510</v>
       </c>
       <c r="F94" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G94" t="s">
         <v>509</v>
@@ -8108,7 +8105,7 @@
         <v>510</v>
       </c>
       <c r="F95" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G95" t="s">
         <v>509</v>
@@ -8134,7 +8131,7 @@
         <v>510</v>
       </c>
       <c r="F96" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G96" t="s">
         <v>509</v>
@@ -8160,7 +8157,7 @@
         <v>510</v>
       </c>
       <c r="F97" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G97" t="s">
         <v>509</v>
@@ -8207,7 +8204,7 @@
         <v>519</v>
       </c>
       <c r="L98" t="s">
-        <v>363</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -8236,7 +8233,7 @@
         <v>519</v>
       </c>
       <c r="L99" t="s">
-        <v>340</v>
+        <v>135</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -8265,7 +8262,7 @@
         <v>519</v>
       </c>
       <c r="L100" t="s">
-        <v>368</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -8308,7 +8305,7 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C102" t="s">
         <v>476</v>
@@ -8337,10 +8334,10 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B103" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D103" t="s">
         <v>129</v>
@@ -8420,23 +8417,26 @@
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>86</v>
+      </c>
       <c r="B106" t="s">
-        <v>178</v>
+        <v>86</v>
       </c>
       <c r="C106" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D106" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E106" t="s">
-        <v>510</v>
+        <v>534</v>
       </c>
       <c r="F106" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="G106" t="s">
-        <v>506</v>
+        <v>544</v>
       </c>
       <c r="H106" t="s">
         <v>511</v>
@@ -8445,106 +8445,106 @@
         <v>545</v>
       </c>
       <c r="J106" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="K106" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="L106" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>86</v>
+        <v>577</v>
       </c>
       <c r="B107" t="s">
-        <v>86</v>
+        <v>577</v>
       </c>
       <c r="C107" t="s">
-        <v>173</v>
+        <v>480</v>
       </c>
       <c r="D107" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="E107" t="s">
         <v>534</v>
       </c>
       <c r="F107" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="G107" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="H107" t="s">
-        <v>511</v>
+        <v>542</v>
       </c>
       <c r="I107" t="s">
-        <v>545</v>
-      </c>
-      <c r="J107" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="K107" t="s">
-        <v>543</v>
+        <v>128</v>
       </c>
       <c r="L107" t="s">
-        <v>543</v>
+        <v>128</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>578</v>
+        <v>70</v>
       </c>
       <c r="B108" t="s">
-        <v>578</v>
+        <v>70</v>
       </c>
       <c r="C108" t="s">
-        <v>480</v>
+        <v>167</v>
       </c>
       <c r="D108" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="E108" t="s">
-        <v>534</v>
+        <v>510</v>
       </c>
       <c r="F108" t="s">
-        <v>540</v>
+        <v>167</v>
       </c>
       <c r="G108" t="s">
-        <v>541</v>
+        <v>508</v>
       </c>
       <c r="H108" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="I108" t="s">
-        <v>540</v>
+        <v>538</v>
+      </c>
+      <c r="J108" t="s">
+        <v>539</v>
       </c>
       <c r="K108" t="s">
-        <v>128</v>
+        <v>537</v>
       </c>
       <c r="L108" t="s">
-        <v>128</v>
+        <v>537</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B109" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C109" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D109" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E109" t="s">
         <v>510</v>
       </c>
       <c r="F109" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G109" t="s">
         <v>508</v>
@@ -8567,22 +8567,22 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B110" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C110" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D110" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E110" t="s">
         <v>510</v>
       </c>
       <c r="F110" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G110" t="s">
         <v>508</v>
@@ -8605,22 +8605,22 @@
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B111" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C111" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D111" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E111" t="s">
         <v>510</v>
       </c>
       <c r="F111" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G111" t="s">
         <v>508</v>
@@ -8643,25 +8643,22 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>78</v>
-      </c>
-      <c r="B112" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C112" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
       <c r="D112" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
       <c r="E112" t="s">
         <v>510</v>
       </c>
       <c r="F112" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
       <c r="G112" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="H112" t="s">
         <v>537</v>
@@ -8681,22 +8678,25 @@
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="B113" t="s">
+        <v>82</v>
       </c>
       <c r="C113" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="D113" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="E113" t="s">
         <v>510</v>
       </c>
       <c r="F113" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="G113" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H113" t="s">
         <v>537</v>
@@ -8715,23 +8715,14 @@
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>82</v>
-      </c>
-      <c r="B114" t="s">
-        <v>82</v>
-      </c>
-      <c r="C114" t="s">
-        <v>174</v>
-      </c>
       <c r="D114" t="s">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="E114" t="s">
         <v>510</v>
       </c>
       <c r="F114" t="s">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="G114" t="s">
         <v>508</v>
@@ -8754,13 +8745,13 @@
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="E115" t="s">
         <v>510</v>
       </c>
       <c r="F115" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="G115" t="s">
         <v>508</v>
@@ -8783,13 +8774,13 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D116" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="E116" t="s">
         <v>510</v>
       </c>
       <c r="F116" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="G116" t="s">
         <v>508</v>
@@ -8811,27 +8802,21 @@
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D117" t="s">
-        <v>211</v>
+      <c r="C117" t="s">
+        <v>484</v>
       </c>
       <c r="E117" t="s">
         <v>510</v>
       </c>
       <c r="F117" t="s">
-        <v>211</v>
+        <v>537</v>
       </c>
       <c r="G117" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H117" t="s">
         <v>537</v>
       </c>
-      <c r="I117" t="s">
-        <v>538</v>
-      </c>
-      <c r="J117" t="s">
-        <v>539</v>
-      </c>
       <c r="K117" t="s">
         <v>537</v>
       </c>
@@ -8840,8 +8825,17 @@
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>74</v>
+      </c>
+      <c r="B118" t="s">
+        <v>74</v>
+      </c>
       <c r="C118" t="s">
-        <v>484</v>
+        <v>479</v>
+      </c>
+      <c r="D118" t="s">
+        <v>171</v>
       </c>
       <c r="E118" t="s">
         <v>510</v>
@@ -8862,43 +8856,11 @@
         <v>537</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>74</v>
-      </c>
-      <c r="B119" t="s">
-        <v>74</v>
-      </c>
-      <c r="C119" t="s">
-        <v>479</v>
-      </c>
-      <c r="D119" t="s">
-        <v>171</v>
-      </c>
-      <c r="E119" t="s">
-        <v>510</v>
-      </c>
-      <c r="F119" t="s">
-        <v>537</v>
-      </c>
-      <c r="G119" t="s">
-        <v>504</v>
-      </c>
-      <c r="H119" t="s">
-        <v>537</v>
-      </c>
-      <c r="K119" t="s">
-        <v>537</v>
-      </c>
-      <c r="L119" t="s">
-        <v>537</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L119">
-    <sortCondition ref="H2:H119"/>
-    <sortCondition ref="I2:I119"/>
-    <sortCondition ref="J2:J119"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L118">
+    <sortCondition ref="H2:H118"/>
+    <sortCondition ref="I2:I118"/>
+    <sortCondition ref="J2:J118"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>